<commit_message>
Se realiza la prime implemenatción de los primeros  formularios
</commit_message>
<xml_diff>
--- a/community-kitchens-front/src/assets/i18n/Lenguaje.xlsx
+++ b/community-kitchens-front/src/assets/i18n/Lenguaje.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Aplicación_Tesis\Community_Kitchens\community-kitchens-front\src\assets\i18n\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tesis\Community_Kitchens\community-kitchens-front\src\assets\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>Code</t>
   </si>
@@ -129,6 +129,108 @@
   </si>
   <si>
     <t>papa</t>
+  </si>
+  <si>
+    <t>Kilo</t>
+  </si>
+  <si>
+    <t>At</t>
+  </si>
+  <si>
+    <t>Gram</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Shooting</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Ton</t>
+  </si>
+  <si>
+    <t>Pipe</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>Reel</t>
+  </si>
+  <si>
+    <t>Strip</t>
+  </si>
+  <si>
+    <t>Roll</t>
+  </si>
+  <si>
+    <t>Milligram</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Ration</t>
+  </si>
+  <si>
+    <t>Arroba</t>
+  </si>
+  <si>
+    <t>Gramo</t>
+  </si>
+  <si>
+    <t>Libra</t>
+  </si>
+  <si>
+    <t>Lote</t>
+  </si>
+  <si>
+    <t>Paquete</t>
+  </si>
+  <si>
+    <t>Disparo</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Tonelada</t>
+  </si>
+  <si>
+    <t>Pipa</t>
+  </si>
+  <si>
+    <t>Barril</t>
+  </si>
+  <si>
+    <t>Carrete</t>
+  </si>
+  <si>
+    <t>Tira</t>
+  </si>
+  <si>
+    <t>Rollo</t>
+  </si>
+  <si>
+    <t>Miligramo</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Ración</t>
   </si>
 </sst>
 </file>
@@ -455,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,11 +616,11 @@
         <v>3</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D14" si="0">CONCATENATE("'",A3,"':","'",B3,"',")</f>
+        <f t="shared" ref="D3:D32" si="0">CONCATENATE("'",A3,"':","'",B3,"',")</f>
         <v>'Name':'Name',</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E14" si="1">CONCATENATE("'",A3,"':","'",C3,"',")</f>
+        <f t="shared" ref="E3:E32" si="1">CONCATENATE("'",A3,"':","'",C3,"',")</f>
         <v>'Name':'Nombre',</v>
       </c>
     </row>
@@ -729,6 +831,348 @@
       <c r="E14" t="str">
         <f t="shared" si="1"/>
         <v>'ZoneReception':'Horario recepción',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>'Kilo':'Kilo',</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>'Kilo':'Kilo',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>'At':'At',</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>'At':'Arroba',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>'Gram':'Gram',</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>'Gram':'Gramo',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>'Pound':'Pound',</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>'Pound':'Libra',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>'Lot':'Lot',</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>'Lot':'Lote',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>'Package':'Package',</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>'Package':'Paquete',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>'Container':'Container',</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>'Container':'Container',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>'Shooting':'Shooting',</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>'Shooting':'Disparo',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>'Group':'Group',</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>'Group':'Grupo',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>'Ton':'Ton',</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>'Ton':'Tonelada',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>'Pipe':'Pipe',</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>'Pipe':'Pipa',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Barrel':'Barrel',</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>'Barrel':'Barril',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>'Reel':'Reel',</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>'Reel':'Carrete',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>'Strip':'Strip',</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>'Strip':'Tira',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>'Roll':'Roll',</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>'Roll':'Rollo',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>'Milligram':'Milligram',</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>'Milligram':'Miligramo',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>'Box':'Box',</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>'Box':'Caja',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>'Ration':'Ration',</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>'Ration':'Ración',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>